<commit_message>
Rest API Get and Post update
</commit_message>
<xml_diff>
--- a/src/main/resources/difference.xlsx
+++ b/src/main/resources/difference.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
   <si>
     <t>id</t>
   </si>
@@ -26,7 +26,7 @@
     <t>price</t>
   </si>
   <si>
-    <t>discountpercentage</t>
+    <t>discountPercentage</t>
   </si>
   <si>
     <t>rating</t>
@@ -47,25 +47,25 @@
     <t>images</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>iPhone X</t>
-  </si>
-  <si>
-    <t>SIM-Free, Model A19211 6.5-inch Super Retina HD display with OLED technology A12 Bionic chip with ...</t>
-  </si>
-  <si>
-    <t>899</t>
-  </si>
-  <si>
-    <t>17.94</t>
-  </si>
-  <si>
-    <t>4.44</t>
-  </si>
-  <si>
-    <t>34</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>iPhone 9</t>
+  </si>
+  <si>
+    <t>An apple mobile which is nothing like apple</t>
+  </si>
+  <si>
+    <t>549</t>
+  </si>
+  <si>
+    <t>12.96</t>
+  </si>
+  <si>
+    <t>4.69</t>
+  </si>
+  <si>
+    <t>94</t>
   </si>
   <si>
     <t>Apple</t>
@@ -74,13 +74,13 @@
     <t>smartphones</t>
   </si>
   <si>
-    <t>https://cdn.dummyjson.com/product-images/2/thumbnail.jpg</t>
-  </si>
-  <si>
-    <t>https://cdn.dummyjson.com/product-images/2/1.jpg, https://cdn.dummyjson.com/product-images/2/2.jpg, https://cdn.dummyjson.com/product-images/2/3.jpg, https://cdn.dummyjson.com/product-images/2/thumbnail.jpg</t>
-  </si>
-  <si>
-    <t>iPhone XX</t>
+    <t>https://i.dummyjson.com/data/products/1/thumbnail.jpg</t>
+  </si>
+  <si>
+    <t>https://i.dummyjson.com/data/products/1/1.jpg, https://i.dummyjson.com/data/products/1/2.jpg, https://i.dummyjson.com/data/products/1/3.jpg, https://i.dummyjson.com/data/products/1/4.jpg, https://i.dummyjson.com/data/products/1/thumbnail.jpg</t>
+  </si>
+  <si>
+    <t>94.86</t>
   </si>
   <si>
     <t>master</t>
@@ -89,37 +89,73 @@
     <t>test</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Samsung Universe 9</t>
-  </si>
-  <si>
-    <t>Samsung's new variant which goes beyond Galaxy to the Universe</t>
-  </si>
-  <si>
-    <t>1249</t>
-  </si>
-  <si>
-    <t>15.46</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Huawei P30</t>
+  </si>
+  <si>
+    <t>Huawei’s re-badged P30 Pro New Edition was officially unveiled yesterday in Germany and now the device has made its way to the UK.</t>
+  </si>
+  <si>
+    <t>499</t>
+  </si>
+  <si>
+    <t>10.58</t>
   </si>
   <si>
     <t>4.09</t>
   </si>
   <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>Samsung</t>
-  </si>
-  <si>
-    <t>https://cdn.dummyjson.com/product-images/3/thumbnail.jpg</t>
-  </si>
-  <si>
-    <t>https://cdn.dummyjson.com/product-images/3/1.jpg</t>
-  </si>
-  <si>
-    <t>SamsungG</t>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Huawei</t>
+  </si>
+  <si>
+    <t>https://i.dummyjson.com/data/products/5/thumbnail.jpg</t>
+  </si>
+  <si>
+    <t>https://i.dummyjson.com/data/products/5/1.jpg, https://i.dummyjson.com/data/products/5/2.jpg, https://i.dummyjson.com/data/products/5/3.jpg</t>
+  </si>
+  <si>
+    <t>4.0955</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Eau De Perfume Spray</t>
+  </si>
+  <si>
+    <t>Genuine  Al-Rehab spray perfume from UAE/Saudi Arabia/Yemen High Quality</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>10.99</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>Lord - Al-Rehab</t>
+  </si>
+  <si>
+    <t>fragrances</t>
+  </si>
+  <si>
+    <t>https://i.dummyjson.com/data/products/15/thumbnail.jpg</t>
+  </si>
+  <si>
+    <t>https://i.dummyjson.com/data/products/15/1.jpg, https://i.dummyjson.com/data/products/15/2.jpg, https://i.dummyjson.com/data/products/15/3.jpg, https://i.dummyjson.com/data/products/15/4.jpg, https://i.dummyjson.com/data/products/15/thumbnail.jpg</t>
+  </si>
+  <si>
+    <t>Genuine  Al-Rehab spray perfume from UAE/Saudi Arabia/Yemen High Qualitydfgd</t>
   </si>
 </sst>
 </file>
@@ -127,13 +163,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -196,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
@@ -206,13 +252,17 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -296,7 +346,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>13</v>
@@ -311,7 +361,7 @@
         <v>16</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s" s="0">
         <v>18</v>
@@ -384,13 +434,13 @@
         <v>29</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s" s="0">
         <v>31</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s" s="0">
         <v>19</v>
@@ -402,6 +452,82 @@
         <v>34</v>
       </c>
       <c r="L5" t="s" s="8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="L6" t="s" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="K7" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="L7" t="s" s="12">
         <v>24</v>
       </c>
     </row>

</xml_diff>